<commit_message>
uploaded hte files from a while
</commit_message>
<xml_diff>
--- a/files/Matières/Emplois du temps/T/Planning_du_12_au_25_04_2021.xlsx
+++ b/files/Matières/Emplois du temps/T/Planning_du_12_au_25_04_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry PC\Documents\001 Github prog Sharing\Backup-of-matiere\files\Matières\Emplois du temps\T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72EA010-41D9-4DD5-BA58-0589BD4E2447}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C208192-C115-485C-8E6E-7879349D7B75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{329A6DB2-6337-4DFF-951B-FC8EC2AB292B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Lundi</t>
   </si>
@@ -133,6 +133,33 @@
   </si>
   <si>
     <t>Allemand</t>
+  </si>
+  <si>
+    <t>Allemand:</t>
+  </si>
+  <si>
+    <t>Leçon: cours du 7 avril</t>
+  </si>
+  <si>
+    <t>Exercices: Sur cahier: Faire les questions 1, 2, 3, 4 du texte B: München bleibt ohne Stolpersteine. voir le document en annexe</t>
+  </si>
+  <si>
+    <t>les documents d'expression orale sur l'axe 1 sont aussi en annexe. Les reprendre et savoir en parler le 28 avril.</t>
+  </si>
+  <si>
+    <t>Réviser les axes 6, 2, 3,</t>
+  </si>
+  <si>
+    <t>axe 6: Wissenschaftlicher Fortschritt und Verantwortungsbewusstsein,</t>
+  </si>
+  <si>
+    <t>axe 2: Privater und öffentlicher Raum,</t>
+  </si>
+  <si>
+    <t>axe 3: Kunst und Raum.</t>
+  </si>
+  <si>
+    <t>Faire une fiche pour chaque axe et faire un résumé des documents vus en cours.</t>
   </si>
 </sst>
 </file>
@@ -648,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC63F00C-3281-49F6-841D-13188AFDAAD8}">
   <dimension ref="A2:AC48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1688,72 +1715,99 @@
       <c r="AB30" s="31"/>
       <c r="AC30" s="31"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="J35" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="J36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="J37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="J38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="J39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="J40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="J41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="J42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="J43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>12</v>
       </c>
@@ -1785,5 +1839,6 @@
     <mergeCell ref="L6:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>